<commit_message>
Funciona todo. CCCN terminado
</commit_message>
<xml_diff>
--- a/data/Tokens_CCCN.xlsx
+++ b/data/Tokens_CCCN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TRABAJO DESARROLLADOR\CCEI_X-X_Biblia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TRABAJO DESARROLLADOR\CCEI_CCCN\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Titulo Preliminar</t>
   </si>
@@ -83,15 +83,9 @@
     <t>Arts_705-723.txt</t>
   </si>
   <si>
-    <t>"&gt; 7000 son 40</t>
-  </si>
-  <si>
     <t>"&gt;" 4000 son 30</t>
   </si>
   <si>
-    <t>INDICE</t>
-  </si>
-  <si>
     <t>Arts_509-528.txt</t>
   </si>
   <si>
@@ -99,6 +93,135 @@
   </si>
   <si>
     <t>Arts_594-637.txt</t>
+  </si>
+  <si>
+    <t>Libro 1</t>
+  </si>
+  <si>
+    <t>Libro II</t>
+  </si>
+  <si>
+    <t>Libro III</t>
+  </si>
+  <si>
+    <t>Titulo 4</t>
+  </si>
+  <si>
+    <t>Titulo 5</t>
+  </si>
+  <si>
+    <t>Arts_724-864.txt</t>
+  </si>
+  <si>
+    <t>Arts_865-956.txt</t>
+  </si>
+  <si>
+    <t>Arts_957-1091.txt</t>
+  </si>
+  <si>
+    <t>Arts_1092-1122.txt</t>
+  </si>
+  <si>
+    <t>Arts_1123-1226.txt</t>
+  </si>
+  <si>
+    <t>Arts_1227-1420.txt</t>
+  </si>
+  <si>
+    <t>Arts_1421-1573.txt</t>
+  </si>
+  <si>
+    <t>Arts_1574-1707.txt</t>
+  </si>
+  <si>
+    <t>Arts_1708-1881.txt</t>
+  </si>
+  <si>
+    <t>Libro IV</t>
+  </si>
+  <si>
+    <t>Arts_1882-1907.txt</t>
+  </si>
+  <si>
+    <t>"&gt; 700 son 40</t>
+  </si>
+  <si>
+    <t>Arts_1908-1940.txt</t>
+  </si>
+  <si>
+    <t>Arts_1941-1982.txt</t>
+  </si>
+  <si>
+    <t>Arts_1983-2036.txt</t>
+  </si>
+  <si>
+    <t>Arts_2037-2072.txt</t>
+  </si>
+  <si>
+    <t>Titulo 6 y 7</t>
+  </si>
+  <si>
+    <t>Arts_2073-2128.txt</t>
+  </si>
+  <si>
+    <t>Titulo 11</t>
+  </si>
+  <si>
+    <t>Titulo 12</t>
+  </si>
+  <si>
+    <t>Titulo 13</t>
+  </si>
+  <si>
+    <t>Titulo 8, 9, 10 y 11</t>
+  </si>
+  <si>
+    <t>Arts_2129-2183.txt</t>
+  </si>
+  <si>
+    <t>Arts_2184-2237.txt</t>
+  </si>
+  <si>
+    <t>Arts_2238-2276.txt</t>
+  </si>
+  <si>
+    <t>Libro V</t>
+  </si>
+  <si>
+    <t>Arts_2277-2315.txt</t>
+  </si>
+  <si>
+    <t>Arts_2316-2362.txt</t>
+  </si>
+  <si>
+    <t>Titulo 5, 6 y 7</t>
+  </si>
+  <si>
+    <t>Titulo 1 ,2,3 y 4</t>
+  </si>
+  <si>
+    <t>Arts_2363-2423.txt</t>
+  </si>
+  <si>
+    <t>Titulo 9 y 10</t>
+  </si>
+  <si>
+    <t>Arts_2424-2461.txt</t>
+  </si>
+  <si>
+    <t>Arts_2462-2531.txt</t>
+  </si>
+  <si>
+    <t>Libro VI</t>
+  </si>
+  <si>
+    <t>Titulo 1, 2 y 3</t>
+  </si>
+  <si>
+    <t>Arts_2594-2671.txt</t>
+  </si>
+  <si>
+    <t>Arts_2532-2593.txt</t>
   </si>
 </sst>
 </file>
@@ -107,7 +230,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -125,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +258,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,19 +302,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -461,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F35"/>
+  <dimension ref="B1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,12 +615,12 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -510,36 +650,27 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9842</v>
-      </c>
-      <c r="E5" s="4">
-        <f>+D5*1.2</f>
-        <v>11810.4</v>
-      </c>
-      <c r="F5" s="5">
-        <v>40</v>
-      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>6155</v>
+        <v>9842</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" ref="E6:E21" si="0">+D6*1.2</f>
-        <v>7386</v>
+        <f>+D6*1.2</f>
+        <v>11810.4</v>
       </c>
       <c r="F6" s="5">
         <v>40</v>
@@ -547,75 +678,79 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="4">
-        <v>2492</v>
+        <v>6155</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>2990.4</v>
+        <f t="shared" ref="E7:E53" si="0">+D7*1.2</f>
+        <v>7386</v>
       </c>
       <c r="F7" s="5">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2492</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>2990.4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>9543</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>11451.6</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F9" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4">
-        <v>4531</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>5437.2</v>
-      </c>
-      <c r="F10" s="5">
-        <v>30</v>
-      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="4">
-        <v>4972</v>
+        <v>4531</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>5966.4</v>
+        <v>5437.2</v>
       </c>
       <c r="F11" s="5">
         <v>30</v>
@@ -623,53 +758,53 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D12" s="4">
-        <v>1564</v>
+        <v>4972</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>1876.8</v>
+        <v>5966.4</v>
       </c>
       <c r="F12" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4">
-        <v>4220</v>
+        <v>1564</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5064</v>
+        <v>1876.8</v>
       </c>
       <c r="F13" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="4">
-        <v>3520</v>
+        <v>4220</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>4224</v>
+        <v>5064</v>
       </c>
       <c r="F14" s="5">
         <v>30</v>
@@ -677,17 +812,17 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D15" s="4">
-        <v>5002</v>
+        <v>3520</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>6002.4</v>
+        <v>4224</v>
       </c>
       <c r="F15" s="5">
         <v>30</v>
@@ -695,143 +830,705 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5002</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>6002.4</v>
+      </c>
+      <c r="F16" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D17" s="4">
         <v>1258</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E17" s="4">
         <f t="shared" si="0"/>
         <v>1509.6</v>
       </c>
-      <c r="F16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4">
+      <c r="F17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4">
-        <f t="shared" si="0"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4">
+        <v>7824</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>9388.7999999999993</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19:F34" si="1">IF(E19&gt;7000,40,IF(E19&gt;3500,30,20))</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4519</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>5422.8</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4">
+        <v>8319</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>9982.7999999999993</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1904</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>2284.7999999999997</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4">
+        <v>7397</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>8876.4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="4">
+        <v>12481</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>14977.199999999999</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="4">
+        <v>11774</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>14128.8</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="4">
+        <v>8717</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="0"/>
+        <v>10460.4</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="4">
+        <v>12209</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
+        <v>14650.8</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7">
+        <f t="shared" ref="E28" si="2">+D28*1.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1695</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1946</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="0"/>
+        <v>2335.1999999999998</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3197</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>3836.3999999999996</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="4">
+        <v>2581</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="0"/>
+        <v>3097.2</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3624</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="0"/>
+        <v>4348.8</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3715</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="0"/>
+        <v>4458</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="4">
+        <v>2977</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="0"/>
+        <v>3572.4</v>
+      </c>
+      <c r="F35" s="8">
+        <f>IF(E35&gt;7000,40,IF(E35&gt;3500,30,20))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="4">
+        <v>3488</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="0"/>
+        <v>4185.5999999999995</v>
+      </c>
+      <c r="F36" s="8">
+        <f t="shared" ref="F36:F53" si="3">IF(E36&gt;7000,40,IF(E36&gt;3500,30,20))</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="4">
+        <v>2951</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="0"/>
+        <v>3541.2</v>
+      </c>
+      <c r="F37" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4">
-        <f t="shared" si="0"/>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="4">
+        <v>2970</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="0"/>
+        <v>3564</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3453</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="0"/>
+        <v>4143.5999999999995</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3553</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="0"/>
+        <v>4263.5999999999995</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2074</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="0"/>
+        <v>2488.7999999999997</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="4">
+        <v>4842</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="0"/>
+        <v>5810.4</v>
+      </c>
+      <c r="F43" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7">
+        <f t="shared" ref="E44" si="4">+D44*1.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="4">
+        <v>3719</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="0"/>
+        <v>4462.8</v>
+      </c>
+      <c r="F45" s="8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="4">
+        <v>6279</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="0"/>
+        <v>7534.7999999999993</v>
+      </c>
+      <c r="F46" s="8">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="2"/>
-      <c r="E23" s="2">
-        <f>SUM(E4:E21)</f>
-        <v>64911.6</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="F47">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="4"/>
+      <c r="E50" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D51" s="4"/>
+      <c r="E51" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="4"/>
+      <c r="E52" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+      <c r="E55" s="2">
+        <f>SUM(E4:E53)</f>
+        <v>218761.19999999998</v>
+      </c>
+      <c r="F55" s="1">
         <v>20046</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="1">
-        <v>20302</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="1">
-        <v>20287</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1004</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="1">
-        <v>20705</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="1">
-        <v>24430</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="1">
-        <v>22911</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="1">
-        <v>20301</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>